<commit_message>
Update and add influenza update
</commit_message>
<xml_diff>
--- a/data/sachsen_kh_normalstation.xlsx
+++ b/data/sachsen_kh_normalstation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\modellclub\2003_covid_modell\_Bulletin\LeipzigPlus_24\IMISE-Epidemiologisches-Bulletin-24\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3822A296-E1C7-4167-9FDC-D8B6F81B580E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BFB228-C6C7-4001-BEE3-6A488F8AA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2136" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2484" windowWidth="17280" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F678"/>
+  <dimension ref="A1:F679"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A675" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C678" sqref="C678:D678"/>
+      <selection activeCell="C679" sqref="C679:D679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9334,7 +9334,7 @@
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="1">
-        <f t="shared" ref="A658:A678" si="0">A657+7</f>
+        <f t="shared" ref="A658:A679" si="0">A657+7</f>
         <v>44789</v>
       </c>
       <c r="B658">
@@ -9644,6 +9644,21 @@
         <v>3</v>
       </c>
       <c r="D678" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A679" s="1">
+        <f t="shared" si="0"/>
+        <v>44936</v>
+      </c>
+      <c r="B679">
+        <v>710</v>
+      </c>
+      <c r="C679" t="s">
+        <v>3</v>
+      </c>
+      <c r="D679" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -9665,6 +9680,7 @@
     <hyperlink ref="D676" r:id="rId9" location="a-8996" display="https://www.coronavirus.sachsen.de/infektionsfaelle-in-sachsen-4151.html#a-8996" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="D677" r:id="rId10" location="a-8996" display="https://www.coronavirus.sachsen.de/infektionsfaelle-in-sachsen-4151.html#a-8996" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D678" r:id="rId11" location="a-8996" display="https://www.coronavirus.sachsen.de/infektionsfaelle-in-sachsen-4151.html#a-8996" xr:uid="{566606F3-88D7-46C7-ABBF-1032490F3859}"/>
+    <hyperlink ref="D679" r:id="rId12" location="a-8996" display="https://www.coronavirus.sachsen.de/infektionsfaelle-in-sachsen-4151.html#a-8996" xr:uid="{03AC2E6D-E849-4012-B4D7-08D15888E4C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>